<commit_message>
Big upload due to problems with uploading to GitHub previously. Mainly changes in R script (starting model selection) and files within Main&CG experiment folder.
</commit_message>
<xml_diff>
--- a/Termites/Precipitation data/Rainfalldata.xlsx
+++ b/Termites/Precipitation data/Rainfalldata.xlsx
@@ -8,20 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansun\Documents\Master data\GitHub__R-stat\AfricanBioServices-Vegetation-and-soils\Termites\Precipitation data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFF8FEC-C503-4C91-AFD9-678529FCABCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387C70BD-E643-4E01-805A-AFA0B784B3BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14016" windowHeight="7212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5352" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3381" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3397" uniqueCount="290">
   <si>
     <t>date.burial</t>
   </si>
@@ -891,13 +896,22 @@
   </si>
   <si>
     <t>Rain.sum</t>
+  </si>
+  <si>
+    <t>Avarage of rain.sum in each region</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Rainfall avarage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -905,13 +919,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -923,10 +974,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -936,9 +990,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="20 % – uthevingsfarge 1" xfId="3" builtinId="30"/>
+    <cellStyle name="God" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Nøytral" xfId="2" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -8874,7 +8934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9B6F3C-DA9A-4BB2-A181-19429E189D73}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -23656,10 +23716,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:B17"/>
+  <dimension ref="A3:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="A3:C23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23673,12 +23733,15 @@
     <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>269</v>
       </c>
@@ -23686,63 +23749,132 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>227</v>
       </c>
       <c r="B5" s="3">
         <v>91.45481084297397</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3">
         <v>162.63420725300006</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E6">
+        <f>AVERAGE(GETPIVOTDATA("rain.sum",$A$3,"area","Handajega","season","Dry"),GETPIVOTDATA("rain.sum",$A$3,"area","Mwantimba","season","Dry"))</f>
+        <v>149.68508834849993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3">
         <v>6.7089623438113177</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7">
+        <f>AVERAGE(GETPIVOTDATA("rain.sum",$A$3,"area","Makao","season","Dry"),GETPIVOTDATA("rain.sum",$A$3,"area","Maswa","season","Dry"))</f>
+        <v>8.2202354184056574</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>9.731508492999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(GETPIVOTDATA("rain.sum",$A$3,"area","Handajega","season","Wet"),GETPIVOTDATA("rain.sum",$A$3,"area","Mwantimba","season","Wet"))</f>
+        <v>195.81464114676558</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>136.73596944399981</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E9">
+        <f>AVERAGE(GETPIVOTDATA("rain.sum",$A$3,"area","Makao","season","Wet"),GETPIVOTDATA("rain.sum",$A$3,"area","Maswa","season","Wet"))</f>
+        <v>196.92556687005964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>171.84818423999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E10">
+        <f>GETPIVOTDATA("rain.sum",$A$3,"area","Seronera","season","Dry")</f>
+        <v>171.84818423999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>228</v>
       </c>
       <c r="B11" s="3">
         <v>196.32705703606038</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E11">
+        <f>GETPIVOTDATA("rain.sum",$A$3,"area","Seronera","season","Wet")</f>
+        <v>175.21589537150001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -23750,7 +23882,7 @@
         <v>184.81193707450004</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
@@ -23758,7 +23890,7 @@
         <v>204.21166114941926</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -23766,7 +23898,7 @@
         <v>189.63947259070002</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -23774,7 +23906,7 @@
         <v>206.81734521903113</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>